<commit_message>
Script para union y variables.
</commit_message>
<xml_diff>
--- a/data/02-df_var_long_revisado.xlsx
+++ b/data/02-df_var_long_revisado.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caayala/Dropbox (DESUC)/Apps/GitHub/desuc_bases_variables/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F239E92-8D83-9F4F-AB1A-3289DFC943FD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BF84D3E-E272-EA4D-B686-3F30736C3511}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28060" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="79">
   <si>
     <t>bicentenario_2015.csv</t>
   </si>
@@ -242,6 +242,21 @@
   </si>
   <si>
     <t>s3_4</t>
+  </si>
+  <si>
+    <t>caso_general</t>
+  </si>
+  <si>
+    <t>tipo</t>
+  </si>
+  <si>
+    <t>t_sexo</t>
+  </si>
+  <si>
+    <t>t_edad</t>
+  </si>
+  <si>
+    <t>t_alzanzado</t>
   </si>
 </sst>
 </file>
@@ -271,12 +286,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -291,9 +312,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -634,304 +658,351 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" customWidth="1"/>
+    <col min="3" max="5" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
+      <c r="B1" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B2" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C3" t="s">
         <v>6</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B4" t="s">
+      <c r="E3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
         <v>0</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>1</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C5" t="s">
         <v>7</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>8</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C6" t="s">
         <v>10</v>
       </c>
       <c r="D6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C7" t="s">
         <v>11</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>7</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>59</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>13</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>14</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>60</v>
       </c>
       <c r="B9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C9" t="s">
         <v>16</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>17</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>61</v>
       </c>
       <c r="B10" t="s">
+        <v>77</v>
+      </c>
+      <c r="C10" t="s">
         <v>19</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>20</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>62</v>
       </c>
       <c r="B11" t="s">
+        <v>78</v>
+      </c>
+      <c r="C11" t="s">
         <v>22</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>23</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>63</v>
       </c>
       <c r="B12" t="s">
+        <v>78</v>
+      </c>
+      <c r="C12" t="s">
         <v>25</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>26</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>64</v>
       </c>
       <c r="B13" t="s">
+        <v>78</v>
+      </c>
+      <c r="C13" t="s">
         <v>28</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>29</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>65</v>
       </c>
       <c r="B14" t="s">
+        <v>78</v>
+      </c>
+      <c r="C14" t="s">
         <v>31</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>32</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>66</v>
       </c>
       <c r="B15" t="s">
+        <v>78</v>
+      </c>
+      <c r="C15" t="s">
         <v>34</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>35</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>67</v>
       </c>
       <c r="B16" t="s">
+        <v>78</v>
+      </c>
+      <c r="C16" t="s">
         <v>37</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>38</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>68</v>
       </c>
       <c r="B17" t="s">
+        <v>78</v>
+      </c>
+      <c r="C17" t="s">
         <v>40</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>41</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>69</v>
       </c>
       <c r="B18" t="s">
+        <v>78</v>
+      </c>
+      <c r="C18" t="s">
         <v>43</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>44</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>70</v>
       </c>
       <c r="B19" t="s">
+        <v>78</v>
+      </c>
+      <c r="C19" t="s">
         <v>46</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>47</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>71</v>
       </c>
       <c r="B20" t="s">
+        <v>78</v>
+      </c>
+      <c r="C20" t="s">
         <v>49</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>50</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>72</v>
       </c>
       <c r="B21" t="s">
+        <v>78</v>
+      </c>
+      <c r="C21" t="s">
         <v>52</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>53</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>73</v>
       </c>
       <c r="B22" t="s">
+        <v>78</v>
+      </c>
+      <c r="C22" t="s">
         <v>55</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>56</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>57</v>
       </c>
     </row>

</xml_diff>